<commit_message>
Add more branches on dispatch chart
</commit_message>
<xml_diff>
--- a/Chart Combination.xlsx
+++ b/Chart Combination.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lisa/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lisa/OneDrive/Reading HARD!!!/Spring 2017/Research Project/figmenta/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,8 @@
     <sheet name="Plot with dim chara" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
     <sheet name="Priority of features" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="7" r:id="rId4"/>
+    <sheet name="Features' Priotity " sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="372">
   <si>
     <t>Box plot</t>
   </si>
@@ -1076,15 +1077,9 @@
     <t>or use 3D</t>
   </si>
   <si>
-    <t>5E, 5F, 5H, 5I dots can not have texture</t>
-  </si>
-  <si>
     <t>use  scatter</t>
   </si>
   <si>
-    <t>L when using DN as a catagorical label</t>
-  </si>
-  <si>
     <t>or use scatter</t>
   </si>
   <si>
@@ -1104,6 +1099,54 @@
   </si>
   <si>
     <t>(tie) 13F 1&amp; 4F requires binning</t>
+  </si>
+  <si>
+    <t>Base Dimension</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>CN (+C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CN + CN </t>
+  </si>
+  <si>
+    <t>CN + CN  + CN</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>For?</t>
+  </si>
+  <si>
+    <t>CN + C + C</t>
+  </si>
+  <si>
+    <t>CN + C</t>
+  </si>
+  <si>
+    <t>Composition</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Comparing</t>
+  </si>
+  <si>
+    <t>Trending</t>
+  </si>
+  <si>
+    <t>for 5E, 5F, 5H, 5I dots can not have texture</t>
+  </si>
+  <si>
+    <t>F when using DN as a catagorical label</t>
+  </si>
+  <si>
+    <t>pp;</t>
   </si>
 </sst>
 </file>
@@ -1163,12 +1206,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1206,7 +1255,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1237,9 +1286,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1267,6 +1313,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1557,8 +1612,8 @@
   <dimension ref="A1:I259"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="92" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="C1:H1"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3890,8 +3945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="107" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showRuler="0" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4164,7 +4219,7 @@
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F21" sqref="F21"/>
+      <selection pane="topRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4175,68 +4230,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="25" t="s">
         <v>331</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
     </row>
     <row r="2" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>355</v>
-      </c>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="16" t="s">
         <v>333</v>
       </c>
     </row>
@@ -4244,7 +4299,7 @@
       <c r="A3" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="24">
         <v>1</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -4253,23 +4308,23 @@
       <c r="D3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="24">
         <v>1</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="H3" s="13">
+        <v>348</v>
+      </c>
+      <c r="H3" s="24">
         <v>1</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K3" s="13">
         <v>1</v>
@@ -4285,7 +4340,7 @@
       <c r="A4" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="24">
         <v>3</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -4294,23 +4349,23 @@
       <c r="D4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="24">
         <v>3</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>335</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="H4" s="13">
+        <v>348</v>
+      </c>
+      <c r="H4" s="24">
         <v>3</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K4" s="13">
         <v>3</v>
@@ -4326,7 +4381,7 @@
       <c r="A5" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="24">
         <v>2</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -4335,23 +4390,23 @@
       <c r="D5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="24">
         <v>2</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>343</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="H5" s="13">
+        <v>348</v>
+      </c>
+      <c r="H5" s="24">
         <v>2</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K5" s="13">
         <v>2</v>
@@ -4489,75 +4544,77 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="9"/>
       <c r="F9" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
-      <c r="D10" s="12"/>
+      <c r="D10" s="26" t="s">
+        <v>371</v>
+      </c>
       <c r="F10" s="10" t="s">
-        <v>350</v>
+        <v>370</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="25" t="s">
         <v>318</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14" t="s">
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25" t="s">
         <v>336</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14" t="s">
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25" t="s">
         <v>337</v>
       </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
       <c r="K11" s="13"/>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="14" t="s">
         <v>344</v>
       </c>
       <c r="M11" s="13"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
-        <v>355</v>
-      </c>
-      <c r="B12" s="16" t="s">
+      <c r="A12" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J12" s="16" t="s">
         <v>333</v>
       </c>
       <c r="K12" s="13"/>
-      <c r="L12" s="18" t="s">
+      <c r="L12" s="17" t="s">
         <v>345</v>
       </c>
       <c r="M12" s="13"/>
@@ -4566,28 +4623,28 @@
       <c r="A13" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="24">
         <v>1</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E13" s="13">
         <v>1</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="18" t="s">
         <v>341</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="27" t="s">
         <v>346</v>
       </c>
       <c r="H13" s="13">
         <v>1</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="18" t="s">
         <v>341</v>
       </c>
       <c r="J13" s="13">
@@ -4601,28 +4658,28 @@
       <c r="A14" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="24">
         <v>4</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E14" s="13">
         <v>3</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="18" t="s">
         <v>341</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="27" t="s">
         <v>346</v>
       </c>
       <c r="H14" s="13">
         <v>3</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="18" t="s">
         <v>341</v>
       </c>
       <c r="J14" s="13">
@@ -4636,65 +4693,65 @@
       <c r="A15" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="24">
         <v>2</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="E15" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="E15" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="20">
         <v>4</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="27" t="s">
         <v>346</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="I15" s="21">
+      <c r="I15" s="20">
         <v>4</v>
       </c>
       <c r="J15" s="13">
         <v>0</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>348</v>
+        <v>369</v>
       </c>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="B16" s="13">
+        <v>352</v>
+      </c>
+      <c r="B16" s="24">
         <v>3</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="E16" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="22">
         <v>1</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="27" t="s">
         <v>346</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="I16" s="24">
+      <c r="I16" s="23">
         <v>1</v>
       </c>
       <c r="J16" s="13">
@@ -4717,19 +4774,19 @@
       <c r="D17" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="21">
         <v>4</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="27" t="s">
         <v>346</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="21">
         <v>4</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="21" t="s">
         <v>340</v>
       </c>
       <c r="J17" s="13">
@@ -4758,7 +4815,7 @@
       <c r="F18" s="13">
         <v>5</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="27" t="s">
         <v>346</v>
       </c>
       <c r="H18" s="13" t="s">
@@ -4789,14 +4846,14 @@
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E22" s="12"/>
       <c r="F22" s="12" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E23" s="12"/>
       <c r="F23" s="12" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G23" s="12"/>
     </row>
@@ -4823,16 +4880,149 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="K1:M1"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="K1:M1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView showRuler="0" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B4" t="s">
+        <v>359</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B5" t="s">
+        <v>360</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B6" t="s">
+        <v>364</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>317</v>
+      </c>
+      <c r="B7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>318</v>
+      </c>
+      <c r="B8" t="s">
+        <v>359</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>319</v>
+      </c>
+      <c r="B9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>